<commit_message>
Calendar had six rows, no sense.
Deleted that sixth row and adjusted cells size to improve readability.
</commit_message>
<xml_diff>
--- a/calendar.xlsx
+++ b/calendar.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Iker\Transportes_SpringBoot\Transportes_spring_boot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2631FE6-D856-4073-BE88-2D56178913DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A1EC436-AA29-49A2-B339-0AE71409F6B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{9D8E8C46-94C0-4136-86B8-3CCA8FE756D3}"/>
   </bookViews>
@@ -75,7 +75,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dddd"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -84,8 +84,14 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
+      <sz val="12.5"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12.7"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
@@ -93,14 +99,29 @@
     </font>
     <font>
       <b/>
-      <sz val="48"/>
+      <sz val="16"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="58"/>
       <color rgb="FF4472C4"/>
       <name val="Seaford"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="12"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -242,37 +263,18 @@
   </cellStyleXfs>
   <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="17" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="17" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="17" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="17" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -283,6 +285,21 @@
     </xf>
     <xf numFmtId="164" fontId="3" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -626,10 +643,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N24"/>
+  <dimension ref="A1:N21"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5:L5"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4:H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -650,410 +667,336 @@
     <col min="14" max="14" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="90.6" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:14" ht="102" customHeight="1" x14ac:dyDescent="1.05">
+      <c r="A1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
     </row>
     <row r="2" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:14" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="13"/>
-      <c r="C3" s="12" t="s">
+      <c r="B3" s="8"/>
+      <c r="C3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="13"/>
-      <c r="E3" s="12" t="s">
+      <c r="D3" s="8"/>
+      <c r="E3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="13"/>
-      <c r="G3" s="12" t="s">
+      <c r="F3" s="8"/>
+      <c r="G3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="13"/>
-      <c r="I3" s="12" t="s">
+      <c r="H3" s="8"/>
+      <c r="I3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="J3" s="14"/>
-      <c r="K3" s="12" t="s">
+      <c r="J3" s="9"/>
+      <c r="K3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="L3" s="13"/>
-      <c r="M3" s="12" t="s">
+      <c r="L3" s="8"/>
+      <c r="M3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="N3" s="13"/>
+      <c r="N3" s="8"/>
     </row>
     <row r="4" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="4"/>
+      <c r="A4" s="10"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="11"/>
     </row>
     <row r="5" spans="1:14" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="9"/>
-      <c r="M5" s="8"/>
-      <c r="N5" s="9"/>
-    </row>
-    <row r="6" spans="1:14" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="2"/>
+      <c r="A5" s="12"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="12"/>
+      <c r="N5" s="13"/>
+    </row>
+    <row r="6" spans="1:14" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="4"/>
     </row>
     <row r="7" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="4"/>
+      <c r="A7" s="10"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="10"/>
+      <c r="N7" s="11"/>
     </row>
     <row r="8" spans="1:14" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="9"/>
-      <c r="M8" s="8"/>
-      <c r="N8" s="9"/>
-    </row>
-    <row r="9" spans="1:14" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="1"/>
-      <c r="N9" s="2"/>
+      <c r="A8" s="12"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="12"/>
+      <c r="N8" s="13"/>
+    </row>
+    <row r="9" spans="1:14" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="4"/>
     </row>
     <row r="10" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="3"/>
-      <c r="N10" s="4"/>
+      <c r="A10" s="10"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="10"/>
+      <c r="N10" s="11"/>
     </row>
     <row r="11" spans="1:14" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="9"/>
-      <c r="M11" s="8"/>
-      <c r="N11" s="9"/>
-    </row>
-    <row r="12" spans="1:14" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="1"/>
-      <c r="N12" s="2"/>
+      <c r="A11" s="12"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="13"/>
+      <c r="M11" s="12"/>
+      <c r="N11" s="13"/>
+    </row>
+    <row r="12" spans="1:14" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="4"/>
     </row>
     <row r="13" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="4"/>
-      <c r="M13" s="3"/>
-      <c r="N13" s="4"/>
+      <c r="A13" s="10"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="11"/>
+      <c r="M13" s="10"/>
+      <c r="N13" s="11"/>
     </row>
     <row r="14" spans="1:14" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="9"/>
-      <c r="K14" s="8"/>
-      <c r="L14" s="9"/>
-      <c r="M14" s="8"/>
-      <c r="N14" s="9"/>
-    </row>
-    <row r="15" spans="1:14" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="1"/>
-      <c r="L15" s="2"/>
-      <c r="M15" s="1"/>
-      <c r="N15" s="2"/>
+      <c r="A14" s="12"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="13"/>
+      <c r="M14" s="12"/>
+      <c r="N14" s="13"/>
+    </row>
+    <row r="15" spans="1:14" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="3"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="4"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="4"/>
     </row>
     <row r="16" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="4"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="4"/>
-      <c r="M16" s="3"/>
-      <c r="N16" s="4"/>
+      <c r="A16" s="10"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="11"/>
+      <c r="M16" s="10"/>
+      <c r="N16" s="11"/>
     </row>
     <row r="17" spans="1:14" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="8"/>
-      <c r="B17" s="9"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="9"/>
-      <c r="K17" s="8"/>
-      <c r="L17" s="9"/>
-      <c r="M17" s="8"/>
-      <c r="N17" s="9"/>
-    </row>
-    <row r="18" spans="1:14" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="1"/>
-      <c r="L18" s="2"/>
-      <c r="M18" s="1"/>
-      <c r="N18" s="2"/>
-    </row>
-    <row r="19" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="4"/>
-      <c r="K19" s="3"/>
-      <c r="L19" s="4"/>
-      <c r="M19" s="3"/>
-      <c r="N19" s="4"/>
-    </row>
-    <row r="20" spans="1:14" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="8"/>
-      <c r="B20" s="9"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="8"/>
-      <c r="J20" s="9"/>
-      <c r="K20" s="8"/>
-      <c r="L20" s="9"/>
-      <c r="M20" s="8"/>
-      <c r="N20" s="9"/>
-    </row>
-    <row r="21" spans="1:14" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="1"/>
-      <c r="L21" s="2"/>
-      <c r="M21" s="1"/>
-      <c r="N21" s="2"/>
-    </row>
-    <row r="22" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="A17" s="12"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="12"/>
+      <c r="L17" s="13"/>
+      <c r="M17" s="12"/>
+      <c r="N17" s="13"/>
+    </row>
+    <row r="18" spans="1:14" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="3"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="4"/>
+    </row>
+    <row r="19" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:14" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="21" spans="1:14" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="134">
-    <mergeCell ref="M11:N11"/>
-    <mergeCell ref="M14:N14"/>
-    <mergeCell ref="K14:L14"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="M16:N16"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="M17:N17"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="K5:L5"/>
+  <mergeCells count="113">
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="I9:J9"/>
     <mergeCell ref="I11:J11"/>
     <mergeCell ref="K11:L11"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="M7:N7"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="M18:N18"/>
+    <mergeCell ref="K18:L18"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="A4:B4"/>
@@ -1069,71 +1012,76 @@
     <mergeCell ref="K3:L3"/>
     <mergeCell ref="K4:L4"/>
     <mergeCell ref="I4:J4"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="M19:N19"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="M21:N21"/>
-    <mergeCell ref="M20:N20"/>
-    <mergeCell ref="K20:L20"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="M18:N18"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="A8:B8"/>
     <mergeCell ref="G7:H7"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="E10:F10"/>
     <mergeCell ref="E7:F7"/>
-    <mergeCell ref="M15:N15"/>
-    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="M14:N14"/>
+    <mergeCell ref="K14:L14"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="M16:N16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="E8:F8"/>
     <mergeCell ref="M9:N9"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="C15:D15"/>
     <mergeCell ref="E15:F15"/>
     <mergeCell ref="G15:H15"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="G9:H9"/>
     <mergeCell ref="G12:H12"/>
     <mergeCell ref="E12:F12"/>
     <mergeCell ref="M10:N10"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="E10:F10"/>
     <mergeCell ref="M13:N13"/>
     <mergeCell ref="G13:H13"/>
     <mergeCell ref="E13:F13"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="M17:N17"/>
     <mergeCell ref="I13:J13"/>
     <mergeCell ref="I12:J12"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="I9:J9"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="To change the starting day of the week, go to cell P12 in About sheet" sqref="A3:B3" xr:uid="{461C8B51-7E29-4CA0-BA6E-690AB7809475}"/>

</xml_diff>

<commit_message>
Calendar needs to have 6 rows
</commit_message>
<xml_diff>
--- a/calendar.xlsx
+++ b/calendar.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Iker\Transportes_SpringBoot\Transportes_spring_boot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A1EC436-AA29-49A2-B339-0AE71409F6B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77D6B654-F0D0-49F5-8454-D2A1BA282B8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{9D8E8C46-94C0-4136-86B8-3CCA8FE756D3}"/>
   </bookViews>
@@ -261,16 +261,40 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="17" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -286,20 +310,20 @@
     <xf numFmtId="164" fontId="3" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -643,10 +667,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N21"/>
+  <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4:H4"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -668,316 +692,382 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="102" customHeight="1" x14ac:dyDescent="1.05">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
     </row>
     <row r="2" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:14" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="7" t="s">
+      <c r="B3" s="16"/>
+      <c r="C3" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="7" t="s">
+      <c r="D3" s="16"/>
+      <c r="E3" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="8"/>
-      <c r="G3" s="7" t="s">
+      <c r="F3" s="16"/>
+      <c r="G3" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="8"/>
-      <c r="I3" s="7" t="s">
+      <c r="H3" s="16"/>
+      <c r="I3" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="J3" s="9"/>
-      <c r="K3" s="7" t="s">
+      <c r="J3" s="17"/>
+      <c r="K3" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="L3" s="8"/>
-      <c r="M3" s="7" t="s">
+      <c r="L3" s="16"/>
+      <c r="M3" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="N3" s="8"/>
+      <c r="N3" s="16"/>
     </row>
     <row r="4" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="10"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="11"/>
-      <c r="M4" s="10"/>
-      <c r="N4" s="11"/>
+      <c r="A4" s="5"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="6"/>
     </row>
     <row r="5" spans="1:14" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="12"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="13"/>
-      <c r="M5" s="12"/>
-      <c r="N5" s="13"/>
+      <c r="A5" s="3"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="4"/>
     </row>
     <row r="6" spans="1:14" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="4"/>
+      <c r="A6" s="7"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="8"/>
     </row>
     <row r="7" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="10"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="11"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="11"/>
-      <c r="M7" s="10"/>
-      <c r="N7" s="11"/>
+      <c r="A7" s="5"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="6"/>
     </row>
     <row r="8" spans="1:14" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="12"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="13"/>
-      <c r="K8" s="12"/>
-      <c r="L8" s="13"/>
-      <c r="M8" s="12"/>
-      <c r="N8" s="13"/>
+      <c r="A8" s="3"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="4"/>
     </row>
     <row r="9" spans="1:14" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="3"/>
-      <c r="N9" s="4"/>
+      <c r="A9" s="7"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="7"/>
+      <c r="N9" s="8"/>
     </row>
     <row r="10" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="10"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="11"/>
-      <c r="K10" s="10"/>
-      <c r="L10" s="11"/>
-      <c r="M10" s="10"/>
-      <c r="N10" s="11"/>
+      <c r="A10" s="5"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="6"/>
     </row>
     <row r="11" spans="1:14" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="12"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="13"/>
-      <c r="K11" s="12"/>
-      <c r="L11" s="13"/>
-      <c r="M11" s="12"/>
-      <c r="N11" s="13"/>
+      <c r="A11" s="3"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="4"/>
     </row>
     <row r="12" spans="1:14" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="4"/>
-      <c r="M12" s="3"/>
-      <c r="N12" s="4"/>
-    </row>
-    <row r="13" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="10"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="11"/>
-      <c r="K13" s="10"/>
-      <c r="L13" s="11"/>
-      <c r="M13" s="10"/>
-      <c r="N13" s="11"/>
+      <c r="A12" s="7"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="8"/>
+    </row>
+    <row r="13" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="5"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="6"/>
     </row>
     <row r="14" spans="1:14" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="12"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="13"/>
-      <c r="K14" s="12"/>
-      <c r="L14" s="13"/>
-      <c r="M14" s="12"/>
-      <c r="N14" s="13"/>
-    </row>
-    <row r="15" spans="1:14" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="4"/>
-      <c r="K15" s="3"/>
-      <c r="L15" s="4"/>
-      <c r="M15" s="3"/>
-      <c r="N15" s="4"/>
-    </row>
-    <row r="16" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="10"/>
-      <c r="B16" s="11"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="10"/>
-      <c r="J16" s="11"/>
-      <c r="K16" s="10"/>
-      <c r="L16" s="11"/>
-      <c r="M16" s="10"/>
-      <c r="N16" s="11"/>
-    </row>
-    <row r="17" spans="1:14" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="12"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="12"/>
-      <c r="J17" s="13"/>
-      <c r="K17" s="12"/>
-      <c r="L17" s="13"/>
-      <c r="M17" s="12"/>
-      <c r="N17" s="13"/>
-    </row>
-    <row r="18" spans="1:14" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="4"/>
-      <c r="K18" s="3"/>
-      <c r="L18" s="4"/>
-      <c r="M18" s="3"/>
-      <c r="N18" s="4"/>
-    </row>
-    <row r="19" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="1:14" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
+      <c r="A14" s="3"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="4"/>
+    </row>
+    <row r="15" spans="1:14" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="7"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="8"/>
+      <c r="M15" s="7"/>
+      <c r="N15" s="8"/>
+    </row>
+    <row r="16" spans="1:14" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="21"/>
+      <c r="B16" s="22"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="21"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="21"/>
+      <c r="J16" s="22"/>
+      <c r="K16" s="21"/>
+      <c r="L16" s="22"/>
+      <c r="M16" s="21"/>
+      <c r="N16" s="22"/>
+    </row>
+    <row r="17" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="19"/>
+      <c r="B17" s="20"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="19"/>
+      <c r="J17" s="20"/>
+      <c r="K17" s="19"/>
+      <c r="L17" s="20"/>
+      <c r="M17" s="19"/>
+      <c r="N17" s="20"/>
+    </row>
+    <row r="18" spans="1:14" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="9"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="12"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="12"/>
+      <c r="M18" s="11"/>
+      <c r="N18" s="12"/>
+    </row>
+    <row r="19" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="5"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="6"/>
+      <c r="M19" s="5"/>
+      <c r="N19" s="6"/>
+    </row>
+    <row r="20" spans="1:14" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="4"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="4"/>
+    </row>
+    <row r="21" spans="1:14" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="7"/>
+      <c r="B21" s="18"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="8"/>
+      <c r="K21" s="7"/>
+      <c r="L21" s="8"/>
+      <c r="M21" s="7"/>
+      <c r="N21" s="8"/>
+    </row>
+    <row r="22" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:14" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
+    <row r="24" spans="1:14" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="113">
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="C18:D18"/>
+  <mergeCells count="134">
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="M16:N16"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="M7:N7"/>
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="C9:D9"/>
@@ -986,17 +1076,23 @@
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="A16:B16"/>
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="M18:N18"/>
-    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="M21:N21"/>
+    <mergeCell ref="K21:L21"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="A4:B4"/>
@@ -1017,26 +1113,6 @@
     <mergeCell ref="K8:L8"/>
     <mergeCell ref="I8:J8"/>
     <mergeCell ref="I5:J5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="M7:N7"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="C5:D5"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="G5:H5"/>
     <mergeCell ref="E9:F9"/>
@@ -1049,13 +1125,18 @@
     <mergeCell ref="K14:L14"/>
     <mergeCell ref="I14:J14"/>
     <mergeCell ref="G14:H14"/>
-    <mergeCell ref="M16:N16"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="G7:H7"/>
     <mergeCell ref="G8:H8"/>
     <mergeCell ref="E8:F8"/>
     <mergeCell ref="M9:N9"/>
@@ -1070,20 +1151,32 @@
     <mergeCell ref="M15:N15"/>
     <mergeCell ref="M12:N12"/>
     <mergeCell ref="E14:F14"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="M17:N17"/>
+    <mergeCell ref="M20:N20"/>
     <mergeCell ref="I13:J13"/>
     <mergeCell ref="I12:J12"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="M18:N18"/>
+    <mergeCell ref="M19:N19"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="K20:L20"/>
+    <mergeCell ref="M17:N17"/>
   </mergeCells>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="To change the starting day of the week, go to cell P12 in About sheet" sqref="A3:B3" xr:uid="{461C8B51-7E29-4CA0-BA6E-690AB7809475}"/>
   </dataValidations>
   <printOptions horizontalCentered="1"/>

</xml_diff>